<commit_message>
Extend lowercase variables to raw-data sources
</commit_message>
<xml_diff>
--- a/data-raw/res1A_focus.xlsx
+++ b/data-raw/res1A_focus.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zurp/Dropbox (Personal)/diss/analy/vid-coding/res1A-focus-hand. done/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zurp/Dropbox (Personal)/diss/analy/vid-coding/res1A-focus. done/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mdg_20171117" sheetId="1" r:id="rId1"/>
     <sheet name="slg_20171117" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,12 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="62">
   <si>
-    <t>Coder</t>
-  </si>
-  <si>
-    <t>Bin</t>
-  </si>
-  <si>
     <t>In</t>
   </si>
   <si>
@@ -224,14 +218,20 @@
     <t>12:51</t>
   </si>
   <si>
-    <t>Code</t>
+    <t>code</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
+  <si>
+    <t>coder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -426,6 +426,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -693,51 +696,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="7" width="5.7109375" customWidth="1"/>
     <col min="9" max="15" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1"/>
@@ -745,21 +746,21 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1"/>
       <c r="I3" s="1"/>
@@ -767,21 +768,21 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1"/>
       <c r="I4" s="1"/>
@@ -789,21 +790,21 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G5" s="1"/>
       <c r="I5" s="1"/>
@@ -811,21 +812,21 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="1"/>
@@ -833,21 +834,21 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G7" s="1"/>
       <c r="I7" s="1"/>
@@ -855,21 +856,21 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="G8" s="1"/>
       <c r="I8" s="1"/>
@@ -877,21 +878,21 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G9" s="1"/>
       <c r="I9" s="1"/>
@@ -899,18 +900,18 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
@@ -921,21 +922,21 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G11" s="1"/>
       <c r="I11" s="1"/>
@@ -943,21 +944,21 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G12" s="1"/>
       <c r="I12" s="1"/>
@@ -965,21 +966,21 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1"/>
       <c r="I13" s="1"/>
@@ -987,21 +988,21 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G14" s="1"/>
       <c r="I14" s="1"/>
@@ -1009,21 +1010,21 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1"/>
       <c r="I15" s="1"/>
@@ -1031,21 +1032,21 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G16" s="1"/>
       <c r="I16" s="1"/>
@@ -1053,21 +1054,21 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G17" s="1"/>
       <c r="I17" s="1"/>
@@ -1075,21 +1076,21 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="G18" s="1"/>
       <c r="I18" s="1"/>
@@ -1097,21 +1098,21 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="G19" s="1"/>
       <c r="I19" s="1"/>
@@ -1119,21 +1120,21 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G20" s="1"/>
       <c r="I20" s="1"/>
@@ -1141,21 +1142,21 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G21" s="1"/>
       <c r="I21" s="1"/>
@@ -1163,21 +1164,21 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="G22" s="1"/>
       <c r="I22" s="1"/>
@@ -1185,21 +1186,21 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G23" s="1"/>
       <c r="I23" s="1"/>
@@ -1207,21 +1208,21 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="G24" s="1"/>
       <c r="I24" s="1"/>
@@ -1229,21 +1230,21 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="G25" s="1"/>
       <c r="I25" s="1"/>
@@ -1252,21 +1253,21 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="G26" s="1"/>
       <c r="I26" s="1"/>
@@ -1275,21 +1276,21 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G27" s="1"/>
       <c r="I27" s="1"/>
@@ -1298,57 +1299,57 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1359,475 +1360,473 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="7" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1" t="s">
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>